<commit_message>
remove sheet "GEO_RNASEQ" from four templates
</commit_message>
<xml_diff>
--- a/templates/dataplant/2EXT01_RNA.xlsx
+++ b/templates/dataplant/2EXT01_RNA.xlsx
@@ -8,14 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/github/nfdi4plants/Swate-templates/templates/dataplant/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AAF6719-D16E-1345-8CE4-A4A2763A8B1A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E46D011-B49F-BB46-8ECD-95BE4636E409}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24260" yWindow="-21100" windowWidth="33080" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-5800" yWindow="-21100" windowWidth="19200" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="rna_extraction" sheetId="1" r:id="rId1"/>
     <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
-    <sheet name="GEO_RNASEQ" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -207,7 +206,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="72">
   <si>
     <t>Source Name</t>
   </si>
@@ -215,24 +214,9 @@
     <t>Sample Name</t>
   </si>
   <si>
-    <t>Parameter [Bio entity]</t>
-  </si>
-  <si>
-    <t>Parameter [Biosource amount]</t>
-  </si>
-  <si>
     <t>Unit</t>
   </si>
   <si>
-    <t>Parameter [Extraction method]</t>
-  </si>
-  <si>
-    <t>Parameter [Extraction buffer]</t>
-  </si>
-  <si>
-    <t>Parameter [Extraction buffer volume]</t>
-  </si>
-  <si>
     <t>Unit (#2)</t>
   </si>
   <si>
@@ -348,111 +332,6 @@
   </si>
   <si>
     <t/>
-  </si>
-  <si>
-    <t>TermSourceRef</t>
-  </si>
-  <si>
-    <t>Ontology</t>
-  </si>
-  <si>
-    <t>TAN</t>
-  </si>
-  <si>
-    <t>Content type (validation)</t>
-  </si>
-  <si>
-    <t>Notes during templating</t>
-  </si>
-  <si>
-    <t>Target term</t>
-  </si>
-  <si>
-    <t>Instruction</t>
-  </si>
-  <si>
-    <t>Requirement (m/o/n)</t>
-  </si>
-  <si>
-    <t>Value (cv/s/d)</t>
-  </si>
-  <si>
-    <t>Additional information</t>
-  </si>
-  <si>
-    <t>Review comments</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000012</t>
-  </si>
-  <si>
-    <t>NFDI4PSO</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000012</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000013</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000013</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000054</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000054</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000050</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000050</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000051</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000051</t>
-  </si>
-  <si>
-    <t>NFDI4PSO:0000062</t>
-  </si>
-  <si>
-    <t>http://purl.obolibrary.org/obo/NFDI4PSO_0000062</t>
-  </si>
-  <si>
-    <t>Unit: microgram</t>
-  </si>
-  <si>
-    <t>Unit: Microliter</t>
-  </si>
-  <si>
-    <t>SAMPLES_molecule</t>
-  </si>
-  <si>
-    <t>Type of molecule that was extracted from the biological material. Include one of the following: total RNA, polyA RNA, cytoplasmic RNA, nuclear RNA, genomic DNA, protein, or other.</t>
-  </si>
-  <si>
-    <t>m</t>
-  </si>
-  <si>
-    <t>cv</t>
-  </si>
-  <si>
-    <t>PROTOCOLS_extract protocol</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Describe the protocols used to extract and prepare the material to be sequenced. </t>
-  </si>
-  <si>
-    <t>o</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>at least some info is required, but not all terms</t>
   </si>
   <si>
     <t>QIAGEN RNEasy</t>
@@ -609,7 +488,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="8">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -687,27 +566,12 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD2D2D2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFD2D2D2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFD2D2D2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFD2D2D2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -741,12 +605,6 @@
     <xf numFmtId="14" fontId="0" fillId="3" borderId="5" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -754,15 +612,6 @@
     <cellStyle name="Normal 3" xfId="1" xr:uid="{F5E1E0D5-7FB4-4F22-8D3C-EFCDC257DFA2}"/>
   </cellStyles>
   <dxfs count="16">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
-    </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.00\ &quot;microliter&quot;"/>
     </dxf>
@@ -802,6 +651,15 @@
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
     </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;milligram&quot;"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
@@ -828,22 +686,22 @@
   <tableColumns count="19">
     <tableColumn id="1" xr3:uid="{DF71AA61-E923-4AAC-A8BA-9D46DCD4BAC1}" name="Source Name"/>
     <tableColumn id="3" xr3:uid="{01CDA9A9-3416-AB47-93ED-08D32CC9AFD5}" name="Parameter [biosource amount]"/>
-    <tableColumn id="4" xr3:uid="{BAC6A063-7015-3F4C-AA31-FE6D4EED5537}" name="Unit" dataDxfId="2"/>
-    <tableColumn id="5" xr3:uid="{DD1D8617-8787-564F-8CD5-3ADC109D95F6}" name="Term Source REF (DPBO:0000013)" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{B4A4946D-047D-A44E-BC9C-012ECBA29F99}" name="Term Accession Number (DPBO:0000013)" dataDxfId="0"/>
-    <tableColumn id="10" xr3:uid="{5B0E65CF-C995-497E-A9B1-46CBAABE7533}" name="Parameter [extraction method]" dataDxfId="15"/>
-    <tableColumn id="11" xr3:uid="{8A603FB3-4968-4A5D-B901-9860EBB49248}" name="Term Source REF (DPBO:0000054)" dataDxfId="14"/>
-    <tableColumn id="12" xr3:uid="{40BF0941-4CDD-4A4A-90EA-105F1A0B0A75}" name="Term Accession Number (DPBO:0000054)" dataDxfId="13"/>
-    <tableColumn id="13" xr3:uid="{C7FECB2E-3E83-4B36-A79A-5DD2E0969A21}" name="Parameter [extraction buffer]" dataDxfId="12"/>
-    <tableColumn id="14" xr3:uid="{4CFA59D3-CCD3-4F3D-A274-03368720E7F7}" name="Term Source REF (DPBO:0000050)" dataDxfId="11"/>
-    <tableColumn id="15" xr3:uid="{CC905BDC-A423-40BD-B9D8-837430F6C524}" name="Term Accession Number (DPBO:0000050)" dataDxfId="10"/>
-    <tableColumn id="16" xr3:uid="{587AE11A-6B65-4A00-A720-B1D3F462F3E9}" name="Parameter [extraction buffer volume]" dataDxfId="9"/>
-    <tableColumn id="17" xr3:uid="{83EC4181-CC19-4F29-A712-25F088C0A200}" name="Unit (#2)" dataDxfId="8"/>
-    <tableColumn id="18" xr3:uid="{C8DB36B5-D383-4FE8-A45D-DE3DFFB70696}" name="Term Source REF (DPBO:0000051)" dataDxfId="7"/>
-    <tableColumn id="19" xr3:uid="{D4A6ACFF-B576-475A-ADA9-56593688C0D2}" name="Term Accession Number (DPBO:0000051)" dataDxfId="6"/>
-    <tableColumn id="20" xr3:uid="{BD9EA8B2-AAD2-413D-B047-B818FDF6F989}" name="Parameter [RNA quality check]" dataDxfId="5"/>
-    <tableColumn id="21" xr3:uid="{CDCB4760-ECBB-46C6-933E-1C2538B373D9}" name="Term Source REF (DPBO:0000062)" dataDxfId="4"/>
-    <tableColumn id="22" xr3:uid="{0B5A8094-8189-4B67-A9E1-E8E9D6761348}" name="Term Accession Number (DPBO:0000062)" dataDxfId="3"/>
+    <tableColumn id="4" xr3:uid="{BAC6A063-7015-3F4C-AA31-FE6D4EED5537}" name="Unit" dataDxfId="15"/>
+    <tableColumn id="5" xr3:uid="{DD1D8617-8787-564F-8CD5-3ADC109D95F6}" name="Term Source REF (DPBO:0000013)" dataDxfId="14"/>
+    <tableColumn id="6" xr3:uid="{B4A4946D-047D-A44E-BC9C-012ECBA29F99}" name="Term Accession Number (DPBO:0000013)" dataDxfId="13"/>
+    <tableColumn id="10" xr3:uid="{5B0E65CF-C995-497E-A9B1-46CBAABE7533}" name="Parameter [extraction method]" dataDxfId="12"/>
+    <tableColumn id="11" xr3:uid="{8A603FB3-4968-4A5D-B901-9860EBB49248}" name="Term Source REF (DPBO:0000054)" dataDxfId="11"/>
+    <tableColumn id="12" xr3:uid="{40BF0941-4CDD-4A4A-90EA-105F1A0B0A75}" name="Term Accession Number (DPBO:0000054)" dataDxfId="10"/>
+    <tableColumn id="13" xr3:uid="{C7FECB2E-3E83-4B36-A79A-5DD2E0969A21}" name="Parameter [extraction buffer]" dataDxfId="9"/>
+    <tableColumn id="14" xr3:uid="{4CFA59D3-CCD3-4F3D-A274-03368720E7F7}" name="Term Source REF (DPBO:0000050)" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{CC905BDC-A423-40BD-B9D8-837430F6C524}" name="Term Accession Number (DPBO:0000050)" dataDxfId="7"/>
+    <tableColumn id="16" xr3:uid="{587AE11A-6B65-4A00-A720-B1D3F462F3E9}" name="Parameter [extraction buffer volume]" dataDxfId="6"/>
+    <tableColumn id="17" xr3:uid="{83EC4181-CC19-4F29-A712-25F088C0A200}" name="Unit (#2)" dataDxfId="5"/>
+    <tableColumn id="18" xr3:uid="{C8DB36B5-D383-4FE8-A45D-DE3DFFB70696}" name="Term Source REF (DPBO:0000051)" dataDxfId="4"/>
+    <tableColumn id="19" xr3:uid="{D4A6ACFF-B576-475A-ADA9-56593688C0D2}" name="Term Accession Number (DPBO:0000051)" dataDxfId="3"/>
+    <tableColumn id="20" xr3:uid="{BD9EA8B2-AAD2-413D-B047-B818FDF6F989}" name="Parameter [RNA quality check]" dataDxfId="2"/>
+    <tableColumn id="21" xr3:uid="{CDCB4760-ECBB-46C6-933E-1C2538B373D9}" name="Term Source REF (DPBO:0000062)" dataDxfId="1"/>
+    <tableColumn id="22" xr3:uid="{0B5A8094-8189-4B67-A9E1-E8E9D6761348}" name="Term Accession Number (DPBO:0000062)" dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{856D9BE2-BD31-4969-93B3-60D776C90AFE}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1179,9 +1037,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="S13" sqref="S13"/>
     </sheetView>
   </sheetViews>
@@ -1216,55 +1074,55 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>108</v>
+        <v>68</v>
       </c>
       <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E1" t="s">
+        <v>59</v>
+      </c>
+      <c r="F1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>70</v>
+      </c>
+      <c r="J1" t="s">
+        <v>62</v>
+      </c>
+      <c r="K1" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" t="s">
+        <v>71</v>
+      </c>
+      <c r="M1" t="s">
+        <v>3</v>
+      </c>
+      <c r="N1" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" t="s">
         <v>4</v>
       </c>
-      <c r="D1" t="s">
-        <v>98</v>
-      </c>
-      <c r="E1" t="s">
-        <v>99</v>
-      </c>
-      <c r="F1" t="s">
-        <v>109</v>
-      </c>
-      <c r="G1" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" t="s">
-        <v>101</v>
-      </c>
-      <c r="I1" t="s">
-        <v>110</v>
-      </c>
-      <c r="J1" t="s">
-        <v>102</v>
-      </c>
-      <c r="K1" t="s">
-        <v>103</v>
-      </c>
-      <c r="L1" t="s">
-        <v>111</v>
-      </c>
-      <c r="M1" t="s">
-        <v>8</v>
-      </c>
-      <c r="N1" t="s">
-        <v>104</v>
-      </c>
-      <c r="O1" t="s">
-        <v>105</v>
-      </c>
-      <c r="P1" t="s">
-        <v>9</v>
-      </c>
       <c r="Q1" t="s">
-        <v>106</v>
+        <v>66</v>
       </c>
       <c r="R1" t="s">
-        <v>107</v>
+        <v>67</v>
       </c>
       <c r="S1" t="s">
         <v>1</v>
@@ -1272,108 +1130,108 @@
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="15" t="s">
-        <v>46</v>
+      <c r="C2" s="13"/>
+      <c r="D2" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>82</v>
+        <v>42</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>84</v>
+        <v>44</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="L2" s="2">
         <v>200</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>86</v>
+        <v>46</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="R2" s="2" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B3" s="1"/>
-      <c r="C3" s="15"/>
-      <c r="D3" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="15" t="s">
-        <v>46</v>
+      <c r="C3" s="13"/>
+      <c r="D3" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>83</v>
+        <v>43</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>85</v>
+        <v>45</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="L3" s="2"/>
       <c r="M3" s="2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>87</v>
+        <v>47</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>88</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B4" s="1"/>
-      <c r="C4" s="15"/>
-      <c r="D4" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E4" s="15" t="s">
-        <v>46</v>
+      <c r="C4" s="13"/>
+      <c r="D4" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
@@ -1383,13 +1241,13 @@
       <c r="K4" s="1"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="N4" s="2" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="O4" s="2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -1397,12 +1255,12 @@
     </row>
     <row r="5" spans="1:19" x14ac:dyDescent="0.2">
       <c r="B5" s="1"/>
-      <c r="C5" s="15"/>
-      <c r="D5" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="E5" s="15" t="s">
-        <v>46</v>
+      <c r="C5" s="13"/>
+      <c r="D5" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>41</v>
       </c>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
@@ -1412,13 +1270,13 @@
       <c r="K5" s="1"/>
       <c r="L5" s="2"/>
       <c r="M5" s="2" t="s">
-        <v>90</v>
+        <v>50</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>89</v>
+        <v>49</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>91</v>
+        <v>51</v>
       </c>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -1436,7 +1294,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8F787C66-F665-436B-AEA3-3426D484FEC5}">
   <dimension ref="A1:E27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
@@ -1448,104 +1306,104 @@
   <sheetData>
     <row r="1" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B1" s="7" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B3" s="12" t="s">
-        <v>92</v>
+        <v>52</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="50" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>35</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>97</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B7" s="9"/>
     </row>
     <row r="8" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B9" s="8"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B10" s="8"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="5" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B11" s="9"/>
     </row>
     <row r="12" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B13" s="8"/>
       <c r="C13" s="8"/>
@@ -1554,7 +1412,7 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1563,98 +1421,98 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="5" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B15" s="9"/>
     </row>
     <row r="16" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B16" s="10" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="B17" s="8" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B21" s="8"/>
       <c r="C21" s="8"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
-        <v>96</v>
+        <v>56</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
-        <v>93</v>
+        <v>53</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>94</v>
+        <v>54</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="6" t="s">
-        <v>95</v>
+        <v>55</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
@@ -1662,327 +1520,6 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:L9"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="34.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.83203125" customWidth="1"/>
-    <col min="9" max="9" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="36.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>47</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>51</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>52</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E2" s="14"/>
-      <c r="F2" s="14"/>
-      <c r="G2" s="14"/>
-      <c r="H2" s="14"/>
-      <c r="I2" s="14"/>
-      <c r="J2" s="14"/>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A3" s="13" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="C3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>46</v>
-      </c>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="14"/>
-      <c r="J3" s="14"/>
-      <c r="K3" s="14"/>
-      <c r="L3" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A4" s="13" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>60</v>
-      </c>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="H4" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="I4" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="J4" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="K4" s="14"/>
-      <c r="L4" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A5" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="C5" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D5" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G5" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H5" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I5" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J5" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K5" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L5" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A6" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="C6" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K6" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L6" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A7" s="13" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="C7" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D7" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K7" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L7" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A8" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="G8" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J8" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K8" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L8" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A9" s="13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="C9" s="14" t="s">
-        <v>59</v>
-      </c>
-      <c r="D9" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="14"/>
-      <c r="G9" s="14" t="s">
-        <v>77</v>
-      </c>
-      <c r="H9" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="I9" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="J9" s="14" t="s">
-        <v>80</v>
-      </c>
-      <c r="K9" s="14" t="s">
-        <v>81</v>
-      </c>
-      <c r="L9" s="14" t="s">
-        <v>46</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>